<commit_message>
wrapping up feature exploration and selection
</commit_message>
<xml_diff>
--- a/featureSelectionNotes.xlsx
+++ b/featureSelectionNotes.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msflo\DSBootcamp\machine-learning-challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076384CC-FA5D-41F1-8140-26DEA8EE2A2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81E44CA-8B8D-44C4-87FC-199A71B6CC9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" activeTab="1" xr2:uid="{A9E436B1-BE40-41E7-82CE-C7157B5F73B6}"/>
+    <workbookView xWindow="375" yWindow="465" windowWidth="22958" windowHeight="12375" activeTab="1" xr2:uid="{A9E436B1-BE40-41E7-82CE-C7157B5F73B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Unscaled Feature Analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Scaled Feature Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Scaled Feature Analysis'!$A$1:$C$50</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="61">
   <si>
     <t>kepid</t>
   </si>
@@ -214,7 +217,10 @@
     <t>Unscaled Evaluation</t>
   </si>
   <si>
-    <t>Scaled Evaluation</t>
+    <t>Overlap Scaled  - False Positive and Confirmed distributions look too similar or overlap too much</t>
+  </si>
+  <si>
+    <t>Selected</t>
   </si>
 </sst>
 </file>
@@ -1128,11 +1134,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A812A2-0AD7-467B-B5DD-4321C5D14472}">
-  <dimension ref="A1:E50"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1140,11 +1147,9 @@
     <col min="1" max="1" width="20.796875" customWidth="1"/>
     <col min="2" max="2" width="17.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -1155,13 +1160,10 @@
         <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1169,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1177,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1185,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1193,7 +1195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1201,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1211,8 +1213,11 @@
       <c r="C7" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1220,7 +1225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1228,7 +1233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1236,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1244,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1252,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1262,8 +1267,11 @@
       <c r="C13" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1271,10 +1279,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1285,7 +1296,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1296,7 +1307,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1307,7 +1318,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1317,8 +1328,11 @@
       <c r="C18" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1326,10 +1340,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1337,10 +1354,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1350,19 +1370,25 @@
       <c r="C21" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1372,8 +1398,11 @@
       <c r="C23" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1381,10 +1410,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1392,10 +1421,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1403,10 +1432,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1416,8 +1445,11 @@
       <c r="C27" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1428,7 +1460,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1439,7 +1471,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1447,10 +1479,10 @@
         <v>0</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1461,7 +1493,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1472,7 +1504,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1482,8 +1514,11 @@
       <c r="C33" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1494,7 +1529,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1505,18 +1540,21 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1527,7 +1565,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1538,7 +1576,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1549,7 +1587,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1560,7 +1598,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1571,7 +1609,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1582,7 +1620,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1593,7 +1631,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1604,7 +1642,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1612,10 +1650,10 @@
         <v>0</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1623,10 +1661,10 @@
         <v>0</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1634,10 +1672,10 @@
         <v>0</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1648,7 +1686,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1659,7 +1697,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1671,6 +1709,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C50" xr:uid="{05CB847C-82EA-40C5-B920-68A8FD9419A6}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>